<commit_message>
Atualiza bases de dados
</commit_message>
<xml_diff>
--- a/reports/repasse_fes.xlsx
+++ b/reports/repasse_fes.xlsx
@@ -466,7 +466,7 @@
         <v>1189731673.32</v>
       </c>
       <c r="G2">
-        <v>1167877665.93</v>
+        <v>1169734603.76</v>
       </c>
       <c r="H2">
         <v>7990805100</v>
@@ -595,7 +595,7 @@
         </is>
       </c>
       <c r="J4">
-        <v>11886761.95627206</v>
+        <v>11986761.95627206</v>
       </c>
       <c r="K4">
         <v>20111231.25</v>
@@ -637,13 +637,13 @@
         <v>37176172.19</v>
       </c>
       <c r="E5">
-        <v>37176172.19</v>
+        <v>12385707.13</v>
       </c>
       <c r="F5">
-        <v>12224740.56</v>
+        <v>6314403.09</v>
       </c>
       <c r="G5">
-        <v>9341437.76</v>
+        <v>4341437.76</v>
       </c>
       <c r="H5">
         <v>7990805100</v>
@@ -654,7 +654,7 @@
         </is>
       </c>
       <c r="J5">
-        <v>51046433.18999996</v>
+        <v>37176172.18999993</v>
       </c>
       <c r="K5">
         <v>9341437.76</v>
@@ -671,7 +671,7 @@
         <v>37176172.19</v>
       </c>
       <c r="O5">
-        <v>24948176.19</v>
+        <v>9342176.19</v>
       </c>
       <c r="P5">
         <v>9341437.860000003</v>
@@ -702,7 +702,7 @@
         <v>85245423.20999999</v>
       </c>
       <c r="G6">
-        <v>82626101.23</v>
+        <v>82632501.23</v>
       </c>
       <c r="H6">
         <v>7990805100</v>
@@ -761,7 +761,7 @@
         <v>393178499.06</v>
       </c>
       <c r="G7">
-        <v>333885740.4</v>
+        <v>342342408.91</v>
       </c>
       <c r="H7">
         <v>7990805100</v>
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="J7">
-        <v>390557590.6737492</v>
+        <v>396545580.0037492</v>
       </c>
       <c r="K7">
         <v>229048236</v>
@@ -820,7 +820,7 @@
         <v>236216405.35</v>
       </c>
       <c r="G8">
-        <v>232956359.52</v>
+        <v>233039239.82</v>
       </c>
       <c r="H8">
         <v>7990805100</v>
@@ -848,7 +848,7 @@
         <v>256013262.6327776</v>
       </c>
       <c r="O8">
-        <v>257849148</v>
+        <v>245610861</v>
       </c>
       <c r="P8">
         <v>245610860.54</v>
@@ -879,7 +879,7 @@
         <v>11433638.63</v>
       </c>
       <c r="G9">
-        <v>11251650.39</v>
+        <v>11240850.39</v>
       </c>
       <c r="H9">
         <v>7990805100</v>
@@ -890,7 +890,7 @@
         </is>
       </c>
       <c r="J9">
-        <v>23268373.36723115</v>
+        <v>17280384.03723116</v>
       </c>
       <c r="K9">
         <v>7090640.64</v>
@@ -907,10 +907,10 @@
         <v>17280384.03723115</v>
       </c>
       <c r="O9">
-        <v>11633133.6</v>
+        <v>11283755.47</v>
       </c>
       <c r="P9">
-        <v>8372808.210000001</v>
+        <v>11251650.39</v>
       </c>
       <c r="Q9">
         <v>7090640.64</v>
@@ -963,7 +963,7 @@
         <v>3334000</v>
       </c>
       <c r="O10">
-        <v>3334000</v>
+        <v>2917300</v>
       </c>
       <c r="P10">
         <v>2917000</v>

</xml_diff>